<commit_message>
Making sure that it has been backed-up. Coming back after two days.
</commit_message>
<xml_diff>
--- a/Step1.xlsx
+++ b/Step1.xlsx
@@ -12,6 +12,9 @@
     <sheet name="TorontoIsland" sheetId="2" r:id="rId3"/>
     <sheet name="London" sheetId="4" r:id="rId4"/>
     <sheet name="Wiarton" sheetId="5" r:id="rId5"/>
+    <sheet name="KW" sheetId="6" r:id="rId6"/>
+    <sheet name="Hamilton" sheetId="7" r:id="rId7"/>
+    <sheet name="Sarnia" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="2">
   <si>
     <t>Date_Time</t>
   </si>
@@ -350,7 +353,7 @@
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="L21" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,7 +772,7 @@
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="F34" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1597,7 +1600,7 @@
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B50"/>
+      <selection activeCell="G26" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1911,7 +1914,7 @@
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F38" sqref="A1:XFD1048576"/>
+      <selection activeCell="B30" sqref="A1:B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2318,4 +2321,1187 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07134482-B971-4888-BDB0-6E42CB79594A}">
+  <dimension ref="A1:B49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="A1:B49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>29675</v>
+      </c>
+      <c r="B2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>41474</v>
+      </c>
+      <c r="B3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>28516</v>
+      </c>
+      <c r="B4">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>39217</v>
+      </c>
+      <c r="B5">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>35625</v>
+      </c>
+      <c r="B6">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>27885</v>
+      </c>
+      <c r="B7">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>36947</v>
+      </c>
+      <c r="B8">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>39928</v>
+      </c>
+      <c r="B9">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>30501</v>
+      </c>
+      <c r="B10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>36110</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>26738</v>
+      </c>
+      <c r="B12">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>27405</v>
+      </c>
+      <c r="B13">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>30802</v>
+      </c>
+      <c r="B14">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>33112</v>
+      </c>
+      <c r="B15">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>39810</v>
+      </c>
+      <c r="B16">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>30313</v>
+      </c>
+      <c r="B17">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>33324</v>
+      </c>
+      <c r="B18">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>36508</v>
+      </c>
+      <c r="B19">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>40592</v>
+      </c>
+      <c r="B20">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>42802</v>
+      </c>
+      <c r="B21">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>31606</v>
+      </c>
+      <c r="B22">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>33920</v>
+      </c>
+      <c r="B23">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>40306</v>
+      </c>
+      <c r="B24">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>31143</v>
+      </c>
+      <c r="B25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>26646</v>
+      </c>
+      <c r="B26">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>27056</v>
+      </c>
+      <c r="B27">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>29231</v>
+      </c>
+      <c r="B28">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>32832</v>
+      </c>
+      <c r="B29">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>35143</v>
+      </c>
+      <c r="B30">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>36636</v>
+      </c>
+      <c r="B31">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>42379</v>
+      </c>
+      <c r="B32">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>28220</v>
+      </c>
+      <c r="B33">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>32457</v>
+      </c>
+      <c r="B34">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>41691</v>
+      </c>
+      <c r="B35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>28949</v>
+      </c>
+      <c r="B36">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>35014</v>
+      </c>
+      <c r="B37">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>34666</v>
+      </c>
+      <c r="B38">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>42104</v>
+      </c>
+      <c r="B39">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>31929</v>
+      </c>
+      <c r="B40">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>43156</v>
+      </c>
+      <c r="B41">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>37548</v>
+      </c>
+      <c r="B42">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>40909</v>
+      </c>
+      <c r="B43">
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B7BCFC-EA2B-4385-A0D4-8AFAFB6CBB13}">
+  <dimension ref="A1:B49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>28516</v>
+      </c>
+      <c r="B2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>26738</v>
+      </c>
+      <c r="B3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>35488</v>
+      </c>
+      <c r="B4">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>28951</v>
+      </c>
+      <c r="B5">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>36110</v>
+      </c>
+      <c r="B6">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>42802</v>
+      </c>
+      <c r="B7">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>27056</v>
+      </c>
+      <c r="B8">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>30802</v>
+      </c>
+      <c r="B9">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>40971</v>
+      </c>
+      <c r="B10">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>29680</v>
+      </c>
+      <c r="B11">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>30044</v>
+      </c>
+      <c r="B12">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>32195</v>
+      </c>
+      <c r="B13">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>35143</v>
+      </c>
+      <c r="B14">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>27846</v>
+      </c>
+      <c r="B15">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>31143</v>
+      </c>
+      <c r="B16">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>41967</v>
+      </c>
+      <c r="B17">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>32715</v>
+      </c>
+      <c r="B18">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>33325</v>
+      </c>
+      <c r="B19">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>28464</v>
+      </c>
+      <c r="B20">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>29231</v>
+      </c>
+      <c r="B21">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>38662</v>
+      </c>
+      <c r="B22">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>39052</v>
+      </c>
+      <c r="B23">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>33772</v>
+      </c>
+      <c r="B24">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>34463</v>
+      </c>
+      <c r="B25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>37752</v>
+      </c>
+      <c r="B26">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>27708</v>
+      </c>
+      <c r="B27">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>31490</v>
+      </c>
+      <c r="B28">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>32898</v>
+      </c>
+      <c r="B29">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>37325</v>
+      </c>
+      <c r="B30">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>41579</v>
+      </c>
+      <c r="B31">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>26323</v>
+      </c>
+      <c r="B32">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>30602</v>
+      </c>
+      <c r="B33">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>39810</v>
+      </c>
+      <c r="B34">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>34977</v>
+      </c>
+      <c r="B35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>39241</v>
+      </c>
+      <c r="B36">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>42115</v>
+      </c>
+      <c r="B37">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>32120</v>
+      </c>
+      <c r="B38">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>36947</v>
+      </c>
+      <c r="B39">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>40250</v>
+      </c>
+      <c r="B40">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>42379</v>
+      </c>
+      <c r="B41">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>40156</v>
+      </c>
+      <c r="B42">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>36523</v>
+      </c>
+      <c r="B43">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>38096</v>
+      </c>
+      <c r="B44">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>43127</v>
+      </c>
+      <c r="B45">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>36529</v>
+      </c>
+      <c r="B46">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>40892</v>
+      </c>
+      <c r="B47">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2335BE7-53E9-49EB-A5A9-C7132C48CC55}">
+  <dimension ref="A1:B49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>28516</v>
+      </c>
+      <c r="B2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>26738</v>
+      </c>
+      <c r="B3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>35488</v>
+      </c>
+      <c r="B4">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>28951</v>
+      </c>
+      <c r="B5">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>36110</v>
+      </c>
+      <c r="B6">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>42802</v>
+      </c>
+      <c r="B7">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>27056</v>
+      </c>
+      <c r="B8">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>30802</v>
+      </c>
+      <c r="B9">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>40971</v>
+      </c>
+      <c r="B10">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>29680</v>
+      </c>
+      <c r="B11">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>30044</v>
+      </c>
+      <c r="B12">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>32195</v>
+      </c>
+      <c r="B13">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>35143</v>
+      </c>
+      <c r="B14">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>27846</v>
+      </c>
+      <c r="B15">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>31143</v>
+      </c>
+      <c r="B16">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>41967</v>
+      </c>
+      <c r="B17">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>32715</v>
+      </c>
+      <c r="B18">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>33325</v>
+      </c>
+      <c r="B19">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>28464</v>
+      </c>
+      <c r="B20">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>29231</v>
+      </c>
+      <c r="B21">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>38662</v>
+      </c>
+      <c r="B22">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>39052</v>
+      </c>
+      <c r="B23">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>33772</v>
+      </c>
+      <c r="B24">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>34463</v>
+      </c>
+      <c r="B25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>37752</v>
+      </c>
+      <c r="B26">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>27708</v>
+      </c>
+      <c r="B27">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>31490</v>
+      </c>
+      <c r="B28">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>32898</v>
+      </c>
+      <c r="B29">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>37325</v>
+      </c>
+      <c r="B30">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>41579</v>
+      </c>
+      <c r="B31">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>26323</v>
+      </c>
+      <c r="B32">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>30602</v>
+      </c>
+      <c r="B33">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>39810</v>
+      </c>
+      <c r="B34">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>34977</v>
+      </c>
+      <c r="B35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>39241</v>
+      </c>
+      <c r="B36">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>42115</v>
+      </c>
+      <c r="B37">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>32120</v>
+      </c>
+      <c r="B38">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>36947</v>
+      </c>
+      <c r="B39">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>40250</v>
+      </c>
+      <c r="B40">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>42379</v>
+      </c>
+      <c r="B41">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>40156</v>
+      </c>
+      <c r="B42">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>36523</v>
+      </c>
+      <c r="B43">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>38096</v>
+      </c>
+      <c r="B44">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>43127</v>
+      </c>
+      <c r="B45">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>36529</v>
+      </c>
+      <c r="B46">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>40892</v>
+      </c>
+      <c r="B47">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Possibly the final version for Wind
</commit_message>
<xml_diff>
--- a/Step1.xlsx
+++ b/Step1.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="2" documentId="5_{CD80CD0F-7332-48B7-B859-9B79BA3C7536}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{25FFE07F-D704-444B-81C9-2F6F8F02882B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{721BB28B-3DF0-4C85-9230-3A36198E2E80}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -770,7 +770,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D844F6-A635-443C-A1FA-7C9B810E0122}">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F34" sqref="A1:XFD1048576"/>
@@ -792,393 +792,513 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>28516</v>
+        <v>21541</v>
       </c>
       <c r="B2">
-        <v>135</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>28951</v>
+        <v>21555</v>
       </c>
       <c r="B3">
-        <v>128</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>28153</v>
+        <v>20780</v>
       </c>
       <c r="B4">
-        <v>119</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>31579</v>
+        <v>23441</v>
       </c>
       <c r="B5">
-        <v>115</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>27846</v>
+        <v>28516</v>
       </c>
       <c r="B6">
-        <v>114</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>33920</v>
+        <v>28951</v>
       </c>
       <c r="B7">
-        <v>111</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>30493</v>
+        <v>24677</v>
       </c>
       <c r="B8">
-        <v>107</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>30313</v>
+        <v>23921</v>
       </c>
       <c r="B9">
-        <v>106</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>29227</v>
+        <v>28153</v>
       </c>
       <c r="B10">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>31143</v>
+        <v>20410</v>
       </c>
       <c r="B11">
-        <v>104</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>34293</v>
+        <v>31579</v>
       </c>
       <c r="B12">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>27708</v>
+        <v>27846</v>
       </c>
       <c r="B13">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>30802</v>
+        <v>21000</v>
       </c>
       <c r="B14">
-        <v>100</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>32516</v>
+        <v>33920</v>
       </c>
       <c r="B15">
-        <v>100</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>41967</v>
+        <v>24885</v>
       </c>
       <c r="B16">
-        <v>100</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>37288</v>
+        <v>30493</v>
       </c>
       <c r="B17">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>38765</v>
+        <v>30313</v>
       </c>
       <c r="B18">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>39678</v>
+        <v>25227</v>
       </c>
       <c r="B19">
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>33572</v>
+        <v>29227</v>
       </c>
       <c r="B20">
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>34666</v>
+        <v>31143</v>
       </c>
       <c r="B21">
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>34793</v>
+        <v>23105</v>
       </c>
       <c r="B22">
-        <v>96</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>35091</v>
+        <v>34293</v>
       </c>
       <c r="B23">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>35483</v>
+        <v>27708</v>
       </c>
       <c r="B24">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>40971</v>
+        <v>30802</v>
       </c>
       <c r="B25">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>27056</v>
+        <v>32516</v>
       </c>
       <c r="B26">
-        <v>93</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>29660</v>
+        <v>41967</v>
       </c>
       <c r="B27">
-        <v>93</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>36932</v>
+        <v>24167</v>
       </c>
       <c r="B28">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>32457</v>
+        <v>37288</v>
       </c>
       <c r="B29">
-        <v>91</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>40661</v>
+        <v>38765</v>
       </c>
       <c r="B30">
-        <v>91</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>26323</v>
+        <v>39678</v>
       </c>
       <c r="B31">
-        <v>90</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>25634</v>
+        <v>21961</v>
       </c>
       <c r="B32">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>26291</v>
+        <v>22653</v>
       </c>
       <c r="B33">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>26738</v>
+        <v>33572</v>
       </c>
       <c r="B34">
-        <v>89</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>36753</v>
+        <v>34666</v>
       </c>
       <c r="B35">
-        <v>89</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>32899</v>
+        <v>34793</v>
       </c>
       <c r="B36">
-        <v>87</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>36110</v>
+        <v>35091</v>
       </c>
       <c r="B37">
-        <v>83</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>37656</v>
+        <v>35483</v>
       </c>
       <c r="B38">
-        <v>82</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>41294</v>
+        <v>40971</v>
       </c>
       <c r="B39">
-        <v>82</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>42746</v>
+        <v>27056</v>
       </c>
       <c r="B40">
-        <v>82</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>36365</v>
+        <v>29660</v>
       </c>
       <c r="B41">
-        <v>80</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>31871</v>
+        <v>36932</v>
       </c>
       <c r="B42">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>38030</v>
+        <v>32457</v>
       </c>
       <c r="B43">
-        <v>76</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>39439</v>
+        <v>40661</v>
       </c>
       <c r="B44">
-        <v>76</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>39883</v>
+        <v>22445</v>
       </c>
       <c r="B45">
-        <v>76</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>42306</v>
+        <v>26323</v>
       </c>
       <c r="B46">
-        <v>76</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>42429</v>
+        <v>25634</v>
       </c>
       <c r="B47">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>38662</v>
+        <v>26291</v>
       </c>
       <c r="B48">
-        <v>72</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>40424</v>
+        <v>26738</v>
       </c>
       <c r="B49">
-        <v>69</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
+        <v>36753</v>
+      </c>
+      <c r="B50">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>32899</v>
+      </c>
+      <c r="B51">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>36110</v>
+      </c>
+      <c r="B52">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>37656</v>
+      </c>
+      <c r="B53">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>41294</v>
+      </c>
+      <c r="B54">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>42746</v>
+      </c>
+      <c r="B55">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>36365</v>
+      </c>
+      <c r="B56">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>31871</v>
+      </c>
+      <c r="B57">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>38030</v>
+      </c>
+      <c r="B58">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>39439</v>
+      </c>
+      <c r="B59">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>39883</v>
+      </c>
+      <c r="B60">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>42306</v>
+      </c>
+      <c r="B61">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>42429</v>
+      </c>
+      <c r="B62">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>38662</v>
+      </c>
+      <c r="B63">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>40424</v>
+      </c>
+      <c r="B64">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
         <v>43123</v>
       </c>
-      <c r="B50">
+      <c r="B65">
         <v>65</v>
       </c>
     </row>
@@ -3130,370 +3250,370 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>28516</v>
+        <v>33324</v>
       </c>
       <c r="B2">
-        <v>133</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>26738</v>
+        <v>36872</v>
       </c>
       <c r="B3">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>35488</v>
+        <v>31816</v>
       </c>
       <c r="B4">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>28951</v>
+        <v>35946</v>
       </c>
       <c r="B5">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>36110</v>
+        <v>29557</v>
       </c>
       <c r="B6">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>42802</v>
+        <v>30802</v>
       </c>
       <c r="B7">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>27056</v>
+        <v>34659</v>
       </c>
       <c r="B8">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>30802</v>
+        <v>30313</v>
       </c>
       <c r="B9">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>40971</v>
+        <v>37324</v>
       </c>
       <c r="B10">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>29680</v>
+        <v>37180</v>
       </c>
       <c r="B11">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>30044</v>
+        <v>28591</v>
       </c>
       <c r="B12">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>32195</v>
+        <v>38295</v>
       </c>
       <c r="B13">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>35143</v>
+        <v>30528</v>
       </c>
       <c r="B14">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>27846</v>
+        <v>36286</v>
       </c>
       <c r="B15">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>31143</v>
+        <v>27224</v>
       </c>
       <c r="B16">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>41967</v>
+        <v>27477</v>
       </c>
       <c r="B17">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>32715</v>
+        <v>35149</v>
       </c>
       <c r="B18">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>33325</v>
+        <v>32832</v>
       </c>
       <c r="B19">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>28464</v>
+        <v>37731</v>
       </c>
       <c r="B20">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>29231</v>
+        <v>29680</v>
       </c>
       <c r="B21">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>38662</v>
+        <v>33617</v>
       </c>
       <c r="B22">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>39052</v>
+        <v>35014</v>
       </c>
       <c r="B23">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>33772</v>
+        <v>35526</v>
       </c>
       <c r="B24">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>34463</v>
+        <v>39928</v>
       </c>
       <c r="B25">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>37752</v>
+        <v>41211</v>
       </c>
       <c r="B26">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>27708</v>
+        <v>29000</v>
       </c>
       <c r="B27">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>31490</v>
+        <v>32898</v>
       </c>
       <c r="B28">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>32898</v>
+        <v>38466</v>
       </c>
       <c r="B29">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>37325</v>
+        <v>31142</v>
       </c>
       <c r="B30">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>41579</v>
+        <v>32232</v>
       </c>
       <c r="B31">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>26323</v>
+        <v>39810</v>
       </c>
       <c r="B32">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>30602</v>
+        <v>27824</v>
       </c>
       <c r="B33">
-        <v>96</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>39810</v>
+        <v>28253</v>
       </c>
       <c r="B34">
-        <v>96</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>34977</v>
+        <v>42445</v>
       </c>
       <c r="B35">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>39241</v>
+        <v>31503</v>
       </c>
       <c r="B36">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>42115</v>
+        <v>42802</v>
       </c>
       <c r="B37">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>32120</v>
+        <v>41943</v>
       </c>
       <c r="B38">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>36947</v>
+        <v>26472</v>
       </c>
       <c r="B39">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>40250</v>
+        <v>39188</v>
       </c>
       <c r="B40">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>42379</v>
+        <v>40525</v>
       </c>
       <c r="B41">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>40156</v>
+        <v>41294</v>
       </c>
       <c r="B42">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>36523</v>
+        <v>26858</v>
       </c>
       <c r="B43">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>38096</v>
+        <v>40747</v>
       </c>
       <c r="B44">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>43127</v>
+        <v>42314</v>
       </c>
       <c r="B45">
-        <v>83</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>36529</v>
+        <v>43112</v>
       </c>
       <c r="B46">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>40892</v>
+        <v>38928</v>
       </c>
       <c r="B47">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>